<commit_message>
Automatic update from (X220-Ableson)
</commit_message>
<xml_diff>
--- a/IntroStats/Module10_Datasets/GrowthHormonesD.xlsx
+++ b/IntroStats/Module10_Datasets/GrowthHormonesD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="14172"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="14175"/>
   </bookViews>
   <sheets>
     <sheet name="GrowthHormonesC" sheetId="1" r:id="rId1"/>
@@ -374,16 +374,16 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -391,7 +391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -399,7 +399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -407,7 +407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -415,7 +415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -423,39 +423,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -463,7 +463,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -471,7 +471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -479,7 +479,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -487,7 +487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -495,7 +495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -503,7 +503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -511,7 +511,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>